<commit_message>
Added a channel-flip to the grids as they were swapped pair-wise
</commit_message>
<xml_diff>
--- a/Tables/Grid_Wire_Channel_Mapping.xlsx
+++ b/Tables/Grid_Wire_Channel_Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGrid/MultiGridMux/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45CA433-17EF-B444-8AFA-DDB17F26C86B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7D675F-B0A4-DC4E-9F3B-26842A4EFA03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5820" yWindow="2420" windowWidth="21820" windowHeight="22120" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
   </bookViews>
@@ -396,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81663BE0-29B8-F646-A110-AC508EA7B182}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,7 +437,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -465,7 +465,7 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -479,7 +479,7 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -493,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -507,7 +507,7 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -521,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -535,7 +535,7 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -549,7 +549,7 @@
         <v>8</v>
       </c>
       <c r="D11">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
         <v>9</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -577,7 +577,7 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -591,7 +591,7 @@
         <v>11</v>
       </c>
       <c r="D14">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
beginning of change to two plots
</commit_message>
<xml_diff>
--- a/Tables/Grid_Wire_Channel_Mapping.xlsx
+++ b/Tables/Grid_Wire_Channel_Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabellejohn/Documents/MultiGridMUX/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29D6E32-CDA2-4D40-8786-92F9E604699E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50971C65-1975-1B46-BA9C-D73B9595C4E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3780" yWindow="460" windowWidth="21820" windowHeight="14480" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
   </bookViews>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81663BE0-29B8-F646-A110-AC508EA7B182}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68:F82"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,7 +472,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -498,7 +498,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -524,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -550,7 +550,7 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -576,7 +576,7 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -602,7 +602,7 @@
         <v>5</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -628,7 +628,7 @@
         <v>6</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G9">
         <v>6</v>
@@ -654,7 +654,7 @@
         <v>7</v>
       </c>
       <c r="F10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G10">
         <v>7</v>
@@ -680,7 +680,7 @@
         <v>8</v>
       </c>
       <c r="F11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11">
         <v>8</v>
@@ -706,7 +706,7 @@
         <v>9</v>
       </c>
       <c r="F12">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G12">
         <v>9</v>
@@ -732,7 +732,7 @@
         <v>10</v>
       </c>
       <c r="F13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G13">
         <v>10</v>
@@ -758,7 +758,7 @@
         <v>11</v>
       </c>
       <c r="F14">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G14">
         <v>11</v>
@@ -778,7 +778,7 @@
         <v>12</v>
       </c>
       <c r="F15">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -792,7 +792,7 @@
         <v>13</v>
       </c>
       <c r="F16">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -806,7 +806,7 @@
         <v>14</v>
       </c>
       <c r="F17">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -820,7 +820,7 @@
         <v>15</v>
       </c>
       <c r="F18">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -834,8 +834,8 @@
         <v>16</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19:F67" si="0">F3+16</f>
-        <v>16</v>
+        <f t="shared" ref="F19:F66" si="0">F3+16</f>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -850,7 +850,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -865,7 +865,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -880,7 +880,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -895,7 +895,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -910,7 +910,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -925,7 +925,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -940,7 +940,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -955,7 +955,7 @@
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -970,7 +970,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -985,7 +985,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1015,7 +1015,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1060,7 +1060,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1135,7 +1135,7 @@
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1299,8 +1299,7 @@
         <v>47</v>
       </c>
       <c r="F50">
-        <f t="shared" si="0"/>
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1314,8 +1313,7 @@
         <v>48</v>
       </c>
       <c r="F51">
-        <f t="shared" si="0"/>
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1329,8 +1327,7 @@
         <v>49</v>
       </c>
       <c r="F52">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1344,8 +1341,7 @@
         <v>50</v>
       </c>
       <c r="F53">
-        <f t="shared" si="0"/>
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1359,8 +1355,7 @@
         <v>51</v>
       </c>
       <c r="F54">
-        <f t="shared" si="0"/>
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1374,8 +1369,7 @@
         <v>52</v>
       </c>
       <c r="F55">
-        <f t="shared" si="0"/>
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -1389,8 +1383,7 @@
         <v>53</v>
       </c>
       <c r="F56">
-        <f t="shared" si="0"/>
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -1404,8 +1397,7 @@
         <v>54</v>
       </c>
       <c r="F57">
-        <f t="shared" si="0"/>
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -1419,8 +1411,7 @@
         <v>55</v>
       </c>
       <c r="F58">
-        <f t="shared" si="0"/>
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -1434,8 +1425,7 @@
         <v>56</v>
       </c>
       <c r="F59">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -1449,8 +1439,7 @@
         <v>57</v>
       </c>
       <c r="F60">
-        <f t="shared" si="0"/>
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -1464,8 +1453,7 @@
         <v>58</v>
       </c>
       <c r="F61">
-        <f t="shared" si="0"/>
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -1479,8 +1467,7 @@
         <v>59</v>
       </c>
       <c r="F62">
-        <f t="shared" si="0"/>
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -1494,8 +1481,7 @@
         <v>60</v>
       </c>
       <c r="F63">
-        <f t="shared" si="0"/>
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -1509,8 +1495,7 @@
         <v>61</v>
       </c>
       <c r="F64">
-        <f t="shared" si="0"/>
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -1524,8 +1509,7 @@
         <v>62</v>
       </c>
       <c r="F65">
-        <f t="shared" si="0"/>
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -1539,8 +1523,7 @@
         <v>63</v>
       </c>
       <c r="F66">
-        <f t="shared" si="0"/>
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -1549,13 +1532,6 @@
       </c>
       <c r="B67">
         <v>19</v>
-      </c>
-      <c r="E67">
-        <v>64</v>
-      </c>
-      <c r="F67">
-        <f t="shared" si="0"/>
-        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated cluster function to separate 20 and 16 layers data
</commit_message>
<xml_diff>
--- a/Tables/Grid_Wire_Channel_Mapping.xlsx
+++ b/Tables/Grid_Wire_Channel_Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabellejohn/Documents/MultiGridMUX/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGrid/MultiGridMux/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29D6E32-CDA2-4D40-8786-92F9E604699E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4A278E-211F-6F49-A0FD-AFD10FEAF630}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="460" windowWidth="21820" windowHeight="14480" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
+    <workbookView xWindow="3780" yWindow="460" windowWidth="21820" windowHeight="16220" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81663BE0-29B8-F646-A110-AC508EA7B182}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68:F82"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,7 +472,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -498,7 +498,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -524,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -550,7 +550,7 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -576,7 +576,7 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -602,7 +602,7 @@
         <v>5</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -628,7 +628,7 @@
         <v>6</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G9">
         <v>6</v>
@@ -654,7 +654,7 @@
         <v>7</v>
       </c>
       <c r="F10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G10">
         <v>7</v>
@@ -680,7 +680,7 @@
         <v>8</v>
       </c>
       <c r="F11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11">
         <v>8</v>
@@ -706,7 +706,7 @@
         <v>9</v>
       </c>
       <c r="F12">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G12">
         <v>9</v>
@@ -732,7 +732,7 @@
         <v>10</v>
       </c>
       <c r="F13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G13">
         <v>10</v>
@@ -758,7 +758,7 @@
         <v>11</v>
       </c>
       <c r="F14">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G14">
         <v>11</v>
@@ -778,7 +778,7 @@
         <v>12</v>
       </c>
       <c r="F15">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -792,7 +792,7 @@
         <v>13</v>
       </c>
       <c r="F16">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -806,7 +806,7 @@
         <v>14</v>
       </c>
       <c r="F17">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -820,7 +820,7 @@
         <v>15</v>
       </c>
       <c r="F18">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -834,8 +834,7 @@
         <v>16</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19:F67" si="0">F3+16</f>
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -849,8 +848,7 @@
         <v>17</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -864,8 +862,7 @@
         <v>18</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -879,8 +876,7 @@
         <v>19</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -894,8 +890,7 @@
         <v>20</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -909,8 +904,7 @@
         <v>21</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -924,8 +918,7 @@
         <v>22</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -939,8 +932,7 @@
         <v>23</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -954,8 +946,7 @@
         <v>24</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -969,8 +960,7 @@
         <v>25</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -984,8 +974,7 @@
         <v>26</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -999,8 +988,7 @@
         <v>27</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1014,8 +1002,7 @@
         <v>28</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1029,8 +1016,7 @@
         <v>29</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1044,8 +1030,7 @@
         <v>30</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1059,8 +1044,7 @@
         <v>31</v>
       </c>
       <c r="F34">
-        <f t="shared" si="0"/>
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1074,8 +1058,7 @@
         <v>32</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1089,8 +1072,7 @@
         <v>33</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1104,8 +1086,7 @@
         <v>34</v>
       </c>
       <c r="F37">
-        <f t="shared" si="0"/>
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1119,8 +1100,7 @@
         <v>35</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1134,8 +1114,7 @@
         <v>36</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1149,8 +1128,7 @@
         <v>37</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1164,8 +1142,7 @@
         <v>38</v>
       </c>
       <c r="F41">
-        <f t="shared" si="0"/>
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1179,8 +1156,7 @@
         <v>39</v>
       </c>
       <c r="F42">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1194,8 +1170,7 @@
         <v>40</v>
       </c>
       <c r="F43">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1209,8 +1184,7 @@
         <v>41</v>
       </c>
       <c r="F44">
-        <f t="shared" si="0"/>
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1224,8 +1198,7 @@
         <v>42</v>
       </c>
       <c r="F45">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1239,8 +1212,7 @@
         <v>43</v>
       </c>
       <c r="F46">
-        <f t="shared" si="0"/>
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1254,8 +1226,7 @@
         <v>44</v>
       </c>
       <c r="F47">
-        <f t="shared" si="0"/>
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1269,8 +1240,7 @@
         <v>45</v>
       </c>
       <c r="F48">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1284,8 +1254,7 @@
         <v>46</v>
       </c>
       <c r="F49">
-        <f t="shared" si="0"/>
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1299,8 +1268,7 @@
         <v>47</v>
       </c>
       <c r="F50">
-        <f t="shared" si="0"/>
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1314,8 +1282,7 @@
         <v>48</v>
       </c>
       <c r="F51">
-        <f t="shared" si="0"/>
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1329,8 +1296,7 @@
         <v>49</v>
       </c>
       <c r="F52">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1344,8 +1310,7 @@
         <v>50</v>
       </c>
       <c r="F53">
-        <f t="shared" si="0"/>
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1359,8 +1324,7 @@
         <v>51</v>
       </c>
       <c r="F54">
-        <f t="shared" si="0"/>
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1374,8 +1338,7 @@
         <v>52</v>
       </c>
       <c r="F55">
-        <f t="shared" si="0"/>
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -1389,8 +1352,7 @@
         <v>53</v>
       </c>
       <c r="F56">
-        <f t="shared" si="0"/>
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -1404,8 +1366,7 @@
         <v>54</v>
       </c>
       <c r="F57">
-        <f t="shared" si="0"/>
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -1419,8 +1380,7 @@
         <v>55</v>
       </c>
       <c r="F58">
-        <f t="shared" si="0"/>
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -1434,7 +1394,6 @@
         <v>56</v>
       </c>
       <c r="F59">
-        <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
@@ -1449,8 +1408,7 @@
         <v>57</v>
       </c>
       <c r="F60">
-        <f t="shared" si="0"/>
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -1464,8 +1422,7 @@
         <v>58</v>
       </c>
       <c r="F61">
-        <f t="shared" si="0"/>
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -1479,8 +1436,7 @@
         <v>59</v>
       </c>
       <c r="F62">
-        <f t="shared" si="0"/>
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -1494,8 +1450,7 @@
         <v>60</v>
       </c>
       <c r="F63">
-        <f t="shared" si="0"/>
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -1509,8 +1464,7 @@
         <v>61</v>
       </c>
       <c r="F64">
-        <f t="shared" si="0"/>
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -1524,8 +1478,7 @@
         <v>62</v>
       </c>
       <c r="F65">
-        <f t="shared" si="0"/>
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -1539,8 +1492,7 @@
         <v>63</v>
       </c>
       <c r="F66">
-        <f t="shared" si="0"/>
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -1549,13 +1501,6 @@
       </c>
       <c r="B67">
         <v>19</v>
-      </c>
-      <c r="E67">
-        <v>64</v>
-      </c>
-      <c r="F67">
-        <f t="shared" si="0"/>
-        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed optimized code bug
</commit_message>
<xml_diff>
--- a/Tables/Grid_Wire_Channel_Mapping.xlsx
+++ b/Tables/Grid_Wire_Channel_Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabellejohn/Documents/MultiGridMUX/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGrid/MultiGridMux/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50971C65-1975-1B46-BA9C-D73B9595C4E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE930F3-B897-444C-8315-CB04496FD319}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="460" windowWidth="21820" windowHeight="14480" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
+    <workbookView xWindow="40" yWindow="660" windowWidth="12140" windowHeight="16040" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81663BE0-29B8-F646-A110-AC508EA7B182}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,7 +460,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -472,7 +472,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -486,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -498,7 +498,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -512,7 +512,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -524,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -538,7 +538,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -550,7 +550,7 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -564,7 +564,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -576,7 +576,7 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -590,7 +590,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -602,7 +602,7 @@
         <v>5</v>
       </c>
       <c r="F8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -616,7 +616,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -628,7 +628,7 @@
         <v>6</v>
       </c>
       <c r="F9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9">
         <v>6</v>
@@ -642,7 +642,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -654,7 +654,7 @@
         <v>7</v>
       </c>
       <c r="F10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G10">
         <v>7</v>
@@ -668,7 +668,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>8</v>
@@ -680,7 +680,7 @@
         <v>8</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11">
         <v>8</v>
@@ -694,7 +694,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>9</v>
@@ -706,7 +706,7 @@
         <v>9</v>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G12">
         <v>9</v>
@@ -720,7 +720,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -732,7 +732,7 @@
         <v>10</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13">
         <v>10</v>
@@ -746,7 +746,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>11</v>
@@ -758,7 +758,7 @@
         <v>11</v>
       </c>
       <c r="F14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G14">
         <v>11</v>
@@ -772,13 +772,13 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <v>12</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -786,13 +786,13 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E16">
         <v>13</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -800,13 +800,13 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E17">
         <v>14</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -814,13 +814,13 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E18">
         <v>15</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -828,14 +828,13 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="E19">
         <v>16</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19:F66" si="0">F3+16</f>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -843,14 +842,13 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="E20">
         <v>17</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -858,14 +856,13 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="E21">
         <v>18</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -873,14 +870,13 @@
         <v>19</v>
       </c>
       <c r="B22">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="E22">
         <v>19</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -888,14 +884,13 @@
         <v>20</v>
       </c>
       <c r="B23">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E23">
         <v>20</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -903,14 +898,14 @@
         <v>21</v>
       </c>
       <c r="B24">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E24">
         <v>21</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <f t="shared" ref="F19:F49" si="0">F8+16</f>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -918,14 +913,13 @@
         <v>22</v>
       </c>
       <c r="B25">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E25">
         <v>22</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -933,14 +927,13 @@
         <v>23</v>
       </c>
       <c r="B26">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E26">
         <v>23</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -948,14 +941,13 @@
         <v>24</v>
       </c>
       <c r="B27">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E27">
         <v>24</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -963,14 +955,13 @@
         <v>25</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E28">
         <v>25</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -978,14 +969,14 @@
         <v>26</v>
       </c>
       <c r="B29">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E29">
         <v>26</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -993,14 +984,14 @@
         <v>27</v>
       </c>
       <c r="B30">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E30">
         <v>27</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1008,14 +999,14 @@
         <v>28</v>
       </c>
       <c r="B31">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E31">
         <v>28</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1023,14 +1014,14 @@
         <v>29</v>
       </c>
       <c r="B32">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E32">
         <v>29</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1038,14 +1029,14 @@
         <v>30</v>
       </c>
       <c r="B33">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E33">
         <v>30</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1053,14 +1044,14 @@
         <v>31</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E34">
         <v>31</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1068,14 +1059,14 @@
         <v>32</v>
       </c>
       <c r="B35">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="E35">
         <v>32</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1083,14 +1074,14 @@
         <v>33</v>
       </c>
       <c r="B36">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E36">
         <v>33</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1098,14 +1089,14 @@
         <v>34</v>
       </c>
       <c r="B37">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="E37">
         <v>34</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1113,14 +1104,14 @@
         <v>35</v>
       </c>
       <c r="B38">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="E38">
         <v>35</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1128,14 +1119,14 @@
         <v>36</v>
       </c>
       <c r="B39">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="E39">
         <v>36</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1143,14 +1134,14 @@
         <v>37</v>
       </c>
       <c r="B40">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="E40">
         <v>37</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1158,14 +1149,14 @@
         <v>38</v>
       </c>
       <c r="B41">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="E41">
         <v>38</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1173,14 +1164,14 @@
         <v>39</v>
       </c>
       <c r="B42">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="E42">
         <v>39</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1188,14 +1179,14 @@
         <v>40</v>
       </c>
       <c r="B43">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E43">
         <v>40</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1203,14 +1194,14 @@
         <v>41</v>
       </c>
       <c r="B44">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E44">
         <v>41</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1218,14 +1209,14 @@
         <v>42</v>
       </c>
       <c r="B45">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E45">
         <v>42</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1233,14 +1224,14 @@
         <v>43</v>
       </c>
       <c r="B46">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E46">
         <v>43</v>
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1248,14 +1239,14 @@
         <v>44</v>
       </c>
       <c r="B47">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E47">
         <v>44</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1263,14 +1254,14 @@
         <v>45</v>
       </c>
       <c r="B48">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E48">
         <v>45</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1278,14 +1269,14 @@
         <v>46</v>
       </c>
       <c r="B49">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E49">
         <v>46</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1293,13 +1284,13 @@
         <v>47</v>
       </c>
       <c r="B50">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E50">
         <v>47</v>
       </c>
       <c r="F50">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1307,13 +1298,13 @@
         <v>48</v>
       </c>
       <c r="B51">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="E51">
         <v>48</v>
       </c>
       <c r="F51">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1321,13 +1312,13 @@
         <v>49</v>
       </c>
       <c r="B52">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="E52">
         <v>49</v>
       </c>
       <c r="F52">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1335,13 +1326,13 @@
         <v>50</v>
       </c>
       <c r="B53">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E53">
         <v>50</v>
       </c>
       <c r="F53">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1349,13 +1340,13 @@
         <v>51</v>
       </c>
       <c r="B54">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="E54">
         <v>51</v>
       </c>
       <c r="F54">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1363,13 +1354,13 @@
         <v>52</v>
       </c>
       <c r="B55">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="E55">
         <v>52</v>
       </c>
       <c r="F55">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -1377,13 +1368,13 @@
         <v>53</v>
       </c>
       <c r="B56">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="E56">
         <v>53</v>
       </c>
       <c r="F56">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -1391,13 +1382,13 @@
         <v>54</v>
       </c>
       <c r="B57">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E57">
         <v>54</v>
       </c>
       <c r="F57">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -1405,13 +1396,13 @@
         <v>55</v>
       </c>
       <c r="B58">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="E58">
         <v>55</v>
       </c>
       <c r="F58">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -1419,13 +1410,13 @@
         <v>56</v>
       </c>
       <c r="B59">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E59">
         <v>56</v>
       </c>
       <c r="F59">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -1433,13 +1424,13 @@
         <v>57</v>
       </c>
       <c r="B60">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E60">
         <v>57</v>
       </c>
       <c r="F60">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -1447,13 +1438,13 @@
         <v>58</v>
       </c>
       <c r="B61">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E61">
         <v>58</v>
       </c>
       <c r="F61">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -1461,13 +1452,13 @@
         <v>59</v>
       </c>
       <c r="B62">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E62">
         <v>59</v>
       </c>
       <c r="F62">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -1475,13 +1466,13 @@
         <v>60</v>
       </c>
       <c r="B63">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E63">
         <v>60</v>
       </c>
       <c r="F63">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -1489,13 +1480,13 @@
         <v>61</v>
       </c>
       <c r="B64">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E64">
         <v>61</v>
       </c>
       <c r="F64">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -1503,13 +1494,13 @@
         <v>62</v>
       </c>
       <c r="B65">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E65">
         <v>62</v>
       </c>
       <c r="F65">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -1517,13 +1508,13 @@
         <v>63</v>
       </c>
       <c r="B66">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E66">
         <v>63</v>
       </c>
       <c r="F66">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -1531,7 +1522,7 @@
         <v>64</v>
       </c>
       <c r="B67">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -1539,7 +1530,7 @@
         <v>65</v>
       </c>
       <c r="B68">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -1547,7 +1538,7 @@
         <v>66</v>
       </c>
       <c r="B69">
-        <v>17</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -1555,7 +1546,7 @@
         <v>67</v>
       </c>
       <c r="B70">
-        <v>16</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -1563,7 +1554,7 @@
         <v>68</v>
       </c>
       <c r="B71">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -1571,7 +1562,7 @@
         <v>69</v>
       </c>
       <c r="B72">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -1579,7 +1570,7 @@
         <v>70</v>
       </c>
       <c r="B73">
-        <v>37</v>
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -1587,7 +1578,7 @@
         <v>71</v>
       </c>
       <c r="B74">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -1595,7 +1586,7 @@
         <v>72</v>
       </c>
       <c r="B75">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -1603,7 +1594,7 @@
         <v>73</v>
       </c>
       <c r="B76">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -1611,7 +1602,7 @@
         <v>74</v>
       </c>
       <c r="B77">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -1619,7 +1610,7 @@
         <v>75</v>
       </c>
       <c r="B78">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -1627,7 +1618,7 @@
         <v>76</v>
       </c>
       <c r="B79">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -1635,7 +1626,7 @@
         <v>77</v>
       </c>
       <c r="B80">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -1643,7 +1634,7 @@
         <v>78</v>
       </c>
       <c r="B81">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -1651,7 +1642,7 @@
         <v>79</v>
       </c>
       <c r="B82">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
old clustering, new plottting
</commit_message>
<xml_diff>
--- a/Tables/Grid_Wire_Channel_Mapping.xlsx
+++ b/Tables/Grid_Wire_Channel_Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabellejohn/Documents/MultiGridMUX/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGrid/MultiGridMux/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50971C65-1975-1B46-BA9C-D73B9595C4E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4516E2E4-2092-8242-A638-A4DACB532B2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="460" windowWidth="21820" windowHeight="14480" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
+    <workbookView xWindow="6080" yWindow="500" windowWidth="12140" windowHeight="16040" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81663BE0-29B8-F646-A110-AC508EA7B182}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,10 +457,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>15</v>
+      </c>
+      <c r="B3">
         <v>0</v>
-      </c>
-      <c r="B3">
-        <v>15</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -469,10 +469,10 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -483,10 +483,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>14</v>
+      </c>
+      <c r="B4">
         <v>1</v>
-      </c>
-      <c r="B4">
-        <v>14</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -495,10 +495,10 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -509,10 +509,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5">
         <v>2</v>
-      </c>
-      <c r="B5">
-        <v>13</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -521,10 +521,10 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -535,10 +535,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
         <v>3</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -547,10 +547,10 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -561,10 +561,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7">
         <v>4</v>
-      </c>
-      <c r="B7">
-        <v>11</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -573,10 +573,10 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -587,10 +587,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
         <v>5</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -599,10 +599,10 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -613,10 +613,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
         <v>6</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -625,10 +625,10 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9">
         <v>6</v>
@@ -639,10 +639,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
         <v>7</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -651,10 +651,10 @@
         <v>6</v>
       </c>
       <c r="E10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G10">
         <v>7</v>
@@ -665,10 +665,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
         <v>8</v>
-      </c>
-      <c r="B11">
-        <v>7</v>
       </c>
       <c r="C11">
         <v>8</v>
@@ -677,10 +677,10 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11">
         <v>8</v>
@@ -691,10 +691,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
         <v>9</v>
-      </c>
-      <c r="B12">
-        <v>6</v>
       </c>
       <c r="C12">
         <v>9</v>
@@ -703,10 +703,10 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G12">
         <v>9</v>
@@ -717,10 +717,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
         <v>10</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -729,10 +729,10 @@
         <v>11</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13">
         <v>10</v>
@@ -743,10 +743,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
         <v>11</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
       </c>
       <c r="C14">
         <v>11</v>
@@ -755,10 +755,10 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G14">
         <v>11</v>
@@ -769,889 +769,880 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
         <v>12</v>
       </c>
-      <c r="B15">
+      <c r="E15">
         <v>3</v>
       </c>
-      <c r="E15">
-        <v>12</v>
-      </c>
       <c r="F15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
         <v>13</v>
       </c>
-      <c r="B16">
+      <c r="E16">
         <v>2</v>
       </c>
-      <c r="E16">
-        <v>13</v>
-      </c>
       <c r="F16">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
         <v>14</v>
       </c>
-      <c r="B17">
+      <c r="E17">
         <v>1</v>
       </c>
-      <c r="E17">
-        <v>14</v>
-      </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
         <v>15</v>
       </c>
-      <c r="B18">
+      <c r="E18">
         <v>0</v>
       </c>
-      <c r="E18">
-        <v>15</v>
-      </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="E19">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19:F66" si="0">F3+16</f>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="E20">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="E21">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B22">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="E22">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B23">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E23">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B24">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E24">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <f t="shared" ref="F24:F49" si="0">F8+16</f>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B25">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E25">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B26">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E26">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B27">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E27">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E28">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B29">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E29">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E30">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E31">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B32">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E32">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B33">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E33">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E34">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B35">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="E35">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B36">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E36">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B37">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="E37">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B38">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="E38">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B39">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="E39">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="E40">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="E41">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B42">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="E42">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B43">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E43">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B44">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E44">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B45">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E45">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B46">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E46">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B47">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E47">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B48">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E48">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B49">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E49">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B50">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E50">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F50">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="E51">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="F51">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B52">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="E52">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F52">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B53">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E53">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F53">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B54">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="E54">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F54">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B55">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="E55">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F55">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B56">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="E56">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F56">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B57">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E57">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F57">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B58">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="E58">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F58">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B59">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E59">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F59">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B60">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E60">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F60">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B61">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E61">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F61">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B62">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E62">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F62">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B63">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E63">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F63">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B64">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E64">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F64">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B65">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E65">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F65">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B66">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E66">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F66">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B67">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B68">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B69">
-        <v>17</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B70">
-        <v>16</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B71">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B72">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B73">
-        <v>37</v>
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B74">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B75">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B76">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B77">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B78">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B79">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B80">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B81">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B82">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new excel file
</commit_message>
<xml_diff>
--- a/Tables/Grid_Wire_Channel_Mapping.xlsx
+++ b/Tables/Grid_Wire_Channel_Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGrid/MultiGridMux/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE930F3-B897-444C-8315-CB04496FD319}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4516E2E4-2092-8242-A638-A4DACB532B2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="660" windowWidth="12140" windowHeight="16040" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
+    <workbookView xWindow="6080" yWindow="500" windowWidth="12140" windowHeight="16040" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81663BE0-29B8-F646-A110-AC508EA7B182}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,7 +457,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -469,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <v>14</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -495,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>15</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -521,7 +521,7 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <v>12</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -547,7 +547,7 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>13</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -573,7 +573,7 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -599,7 +599,7 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F8">
         <v>11</v>
@@ -613,7 +613,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -625,7 +625,7 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -651,7 +651,7 @@
         <v>6</v>
       </c>
       <c r="E10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -677,7 +677,7 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11">
         <v>6</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>9</v>
@@ -703,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F12">
         <v>7</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>10</v>
@@ -729,7 +729,7 @@
         <v>11</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>11</v>
@@ -755,7 +755,7 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -769,13 +769,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B15">
         <v>12</v>
       </c>
       <c r="E15">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F15">
         <v>2</v>
@@ -783,13 +783,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B16">
         <v>13</v>
       </c>
       <c r="E16">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -797,13 +797,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B17">
         <v>14</v>
       </c>
       <c r="E17">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -811,13 +811,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B18">
         <v>15</v>
       </c>
       <c r="E18">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -825,13 +825,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>76</v>
       </c>
       <c r="E19">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F19">
         <v>30</v>
@@ -839,13 +839,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>77</v>
       </c>
       <c r="E20">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F20">
         <v>31</v>
@@ -853,13 +853,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21">
         <v>78</v>
       </c>
       <c r="E21">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F21">
         <v>28</v>
@@ -867,13 +867,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>79</v>
       </c>
       <c r="E22">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F22">
         <v>29</v>
@@ -881,13 +881,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>16</v>
       </c>
       <c r="E23">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F23">
         <v>26</v>
@@ -895,28 +895,28 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>17</v>
       </c>
       <c r="E24">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F19:F49" si="0">F8+16</f>
+        <f t="shared" ref="F24:F49" si="0">F8+16</f>
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>18</v>
       </c>
       <c r="E25">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F25">
         <v>24</v>
@@ -924,13 +924,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B26">
         <v>19</v>
       </c>
       <c r="E26">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F26">
         <v>25</v>
@@ -938,13 +938,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B27">
         <v>20</v>
       </c>
       <c r="E27">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F27">
         <v>22</v>
@@ -952,13 +952,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>21</v>
       </c>
       <c r="E28">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F28">
         <v>23</v>
@@ -966,13 +966,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>22</v>
       </c>
       <c r="E29">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
@@ -981,13 +981,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>23</v>
       </c>
       <c r="E30">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
@@ -996,13 +996,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31">
         <v>24</v>
       </c>
       <c r="E31">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
@@ -1011,13 +1011,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B32">
         <v>25</v>
       </c>
       <c r="E32">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
@@ -1026,13 +1026,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B33">
         <v>26</v>
       </c>
       <c r="E33">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
@@ -1041,13 +1041,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B34">
         <v>27</v>
       </c>
       <c r="E34">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B35">
         <v>28</v>
       </c>
       <c r="E35">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
@@ -1071,13 +1071,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B36">
         <v>29</v>
       </c>
       <c r="E36">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
@@ -1086,13 +1086,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B37">
         <v>30</v>
       </c>
       <c r="E37">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
@@ -1101,13 +1101,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B38">
         <v>31</v>
       </c>
       <c r="E38">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
@@ -1116,13 +1116,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B39">
         <v>72</v>
       </c>
       <c r="E39">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
@@ -1131,13 +1131,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>73</v>
       </c>
       <c r="E40">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
@@ -1146,13 +1146,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41">
         <v>74</v>
       </c>
       <c r="E41">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
@@ -1161,13 +1161,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B42">
         <v>75</v>
       </c>
       <c r="E42">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
@@ -1176,13 +1176,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B43">
         <v>32</v>
       </c>
       <c r="E43">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
@@ -1191,13 +1191,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B44">
         <v>33</v>
       </c>
       <c r="E44">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
@@ -1206,13 +1206,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B45">
         <v>34</v>
       </c>
       <c r="E45">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
@@ -1221,13 +1221,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B46">
         <v>35</v>
       </c>
       <c r="E46">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
@@ -1236,13 +1236,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B47">
         <v>36</v>
       </c>
       <c r="E47">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
@@ -1251,13 +1251,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <v>37</v>
       </c>
       <c r="E48">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B49">
         <v>38</v>
       </c>
       <c r="E49">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
@@ -1281,13 +1281,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>39</v>
       </c>
       <c r="E50">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F50">
         <v>33</v>
@@ -1295,13 +1295,13 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51">
         <v>40</v>
       </c>
       <c r="E51">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="F51">
         <v>62</v>
@@ -1309,13 +1309,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B52">
         <v>41</v>
       </c>
       <c r="E52">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F52">
         <v>63</v>
@@ -1323,13 +1323,13 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B53">
         <v>42</v>
       </c>
       <c r="E53">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F53">
         <v>60</v>
@@ -1337,13 +1337,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B54">
         <v>43</v>
       </c>
       <c r="E54">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F54">
         <v>61</v>
@@ -1351,13 +1351,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B55">
         <v>44</v>
       </c>
       <c r="E55">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F55">
         <v>58</v>
@@ -1365,13 +1365,13 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B56">
         <v>45</v>
       </c>
       <c r="E56">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F56">
         <v>59</v>
@@ -1379,13 +1379,13 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B57">
         <v>46</v>
       </c>
       <c r="E57">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F57">
         <v>56</v>
@@ -1393,13 +1393,13 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B58">
         <v>47</v>
       </c>
       <c r="E58">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F58">
         <v>57</v>
@@ -1407,13 +1407,13 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B59">
         <v>68</v>
       </c>
       <c r="E59">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F59">
         <v>54</v>
@@ -1421,13 +1421,13 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>69</v>
       </c>
       <c r="E60">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F60">
         <v>55</v>
@@ -1435,13 +1435,13 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B61">
         <v>70</v>
       </c>
       <c r="E61">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F61">
         <v>52</v>
@@ -1449,13 +1449,13 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B62">
         <v>71</v>
       </c>
       <c r="E62">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F62">
         <v>53</v>
@@ -1463,13 +1463,13 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B63">
         <v>48</v>
       </c>
       <c r="E63">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F63">
         <v>50</v>
@@ -1477,13 +1477,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B64">
         <v>49</v>
       </c>
       <c r="E64">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F64">
         <v>51</v>
@@ -1491,13 +1491,13 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B65">
         <v>50</v>
       </c>
       <c r="E65">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F65">
         <v>48</v>
@@ -1505,13 +1505,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B66">
         <v>51</v>
       </c>
       <c r="E66">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F66">
         <v>49</v>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B67">
         <v>52</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B68">
         <v>53</v>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B69">
         <v>54</v>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B70">
         <v>55</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B71">
         <v>56</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B72">
         <v>57</v>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B73">
         <v>58</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B74">
         <v>59</v>
@@ -1583,7 +1583,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B75">
         <v>60</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B76">
         <v>61</v>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B77">
         <v>62</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B78">
         <v>63</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B79">
         <v>64</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B80">
         <v>65</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B81">
         <v>66</v>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B82">
         <v>67</v>

</xml_diff>

<commit_message>
Changed the mapping and mirrored the row numbering
</commit_message>
<xml_diff>
--- a/Tables/Grid_Wire_Channel_Mapping.xlsx
+++ b/Tables/Grid_Wire_Channel_Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGrid/MultiGridMux/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4516E2E4-2092-8242-A638-A4DACB532B2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4320A5-F7BA-C741-A07F-EF9D8996978E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="500" windowWidth="12140" windowHeight="16040" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="17100" windowHeight="16260" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81663BE0-29B8-F646-A110-AC508EA7B182}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,7 +457,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -469,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>14</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -495,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>15</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -521,7 +521,7 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <v>12</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -547,7 +547,7 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>13</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -573,7 +573,7 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -599,7 +599,7 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <v>11</v>
@@ -613,7 +613,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -625,7 +625,7 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -651,7 +651,7 @@
         <v>6</v>
       </c>
       <c r="E10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -677,7 +677,7 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11">
         <v>6</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>9</v>
@@ -703,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>7</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>10</v>
@@ -729,7 +729,7 @@
         <v>11</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>11</v>
@@ -755,7 +755,7 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -769,13 +769,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>12</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F15">
         <v>2</v>
@@ -783,13 +783,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>13</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -797,13 +797,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>14</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -811,13 +811,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>15</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -825,13 +825,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B19">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E19">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F19">
         <v>30</v>
@@ -839,13 +839,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E20">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F20">
         <v>31</v>
@@ -853,13 +853,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E21">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F21">
         <v>28</v>
@@ -867,13 +867,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B22">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E22">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F22">
         <v>29</v>
@@ -881,13 +881,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>16</v>
       </c>
       <c r="E23">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F23">
         <v>26</v>
@@ -895,13 +895,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B24">
         <v>17</v>
       </c>
       <c r="E24">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F24">
         <f t="shared" ref="F24:F49" si="0">F8+16</f>
@@ -910,13 +910,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>18</v>
       </c>
       <c r="E25">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F25">
         <v>24</v>
@@ -924,13 +924,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>19</v>
       </c>
       <c r="E26">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F26">
         <v>25</v>
@@ -938,13 +938,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>20</v>
       </c>
       <c r="E27">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F27">
         <v>22</v>
@@ -952,13 +952,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B28">
         <v>21</v>
       </c>
       <c r="E28">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F28">
         <v>23</v>
@@ -966,13 +966,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>22</v>
       </c>
       <c r="E29">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
@@ -981,13 +981,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30">
         <v>23</v>
       </c>
       <c r="E30">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
@@ -996,13 +996,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B31">
         <v>24</v>
       </c>
       <c r="E31">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
@@ -1011,13 +1011,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B32">
         <v>25</v>
       </c>
       <c r="E32">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
@@ -1026,13 +1026,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B33">
         <v>26</v>
       </c>
       <c r="E33">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
@@ -1041,13 +1041,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B34">
         <v>27</v>
       </c>
       <c r="E34">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B35">
         <v>28</v>
       </c>
       <c r="E35">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
@@ -1071,13 +1071,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B36">
         <v>29</v>
       </c>
       <c r="E36">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
@@ -1086,13 +1086,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B37">
         <v>30</v>
       </c>
       <c r="E37">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
@@ -1101,13 +1101,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B38">
         <v>31</v>
       </c>
       <c r="E38">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
@@ -1116,13 +1116,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B39">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E39">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
@@ -1131,13 +1131,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E40">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
@@ -1146,13 +1146,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B41">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E41">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
@@ -1161,13 +1161,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B42">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E42">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
@@ -1176,13 +1176,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B43">
         <v>32</v>
       </c>
       <c r="E43">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
@@ -1191,13 +1191,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B44">
         <v>33</v>
       </c>
       <c r="E44">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
@@ -1206,13 +1206,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B45">
         <v>34</v>
       </c>
       <c r="E45">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
@@ -1221,13 +1221,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B46">
         <v>35</v>
       </c>
       <c r="E46">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
@@ -1236,13 +1236,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B47">
         <v>36</v>
       </c>
       <c r="E47">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
@@ -1251,13 +1251,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B48">
         <v>37</v>
       </c>
       <c r="E48">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B49">
         <v>38</v>
       </c>
       <c r="E49">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
@@ -1281,13 +1281,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50">
         <v>39</v>
       </c>
       <c r="E50">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F50">
         <v>33</v>
@@ -1295,13 +1295,13 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B51">
         <v>40</v>
       </c>
       <c r="E51">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F51">
         <v>62</v>
@@ -1309,13 +1309,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B52">
         <v>41</v>
       </c>
       <c r="E52">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F52">
         <v>63</v>
@@ -1323,13 +1323,13 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B53">
         <v>42</v>
       </c>
       <c r="E53">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F53">
         <v>60</v>
@@ -1337,13 +1337,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B54">
         <v>43</v>
       </c>
       <c r="E54">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F54">
         <v>61</v>
@@ -1351,13 +1351,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B55">
         <v>44</v>
       </c>
       <c r="E55">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F55">
         <v>58</v>
@@ -1365,13 +1365,13 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B56">
         <v>45</v>
       </c>
       <c r="E56">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F56">
         <v>59</v>
@@ -1379,13 +1379,13 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B57">
         <v>46</v>
       </c>
       <c r="E57">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F57">
         <v>56</v>
@@ -1393,13 +1393,13 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B58">
         <v>47</v>
       </c>
       <c r="E58">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F58">
         <v>57</v>
@@ -1407,13 +1407,13 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B59">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E59">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F59">
         <v>54</v>
@@ -1421,13 +1421,13 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E60">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F60">
         <v>55</v>
@@ -1435,13 +1435,13 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B61">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E61">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F61">
         <v>52</v>
@@ -1449,13 +1449,13 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B62">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E62">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F62">
         <v>53</v>
@@ -1463,13 +1463,13 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B63">
         <v>48</v>
       </c>
       <c r="E63">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F63">
         <v>50</v>
@@ -1477,13 +1477,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B64">
         <v>49</v>
       </c>
       <c r="E64">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F64">
         <v>51</v>
@@ -1491,13 +1491,13 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B65">
         <v>50</v>
       </c>
       <c r="E65">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F65">
         <v>48</v>
@@ -1505,13 +1505,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B66">
         <v>51</v>
       </c>
       <c r="E66">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="F66">
         <v>49</v>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B67">
         <v>52</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B68">
         <v>53</v>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B69">
         <v>54</v>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70">
         <v>55</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B71">
         <v>56</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B72">
         <v>57</v>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B73">
         <v>58</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B74">
         <v>59</v>
@@ -1583,7 +1583,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B75">
         <v>60</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B76">
         <v>61</v>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B77">
         <v>62</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B78">
         <v>63</v>
@@ -1615,34 +1615,34 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B79">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B81">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B82">
-        <v>67</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed error with 13 grids instead of 12, changed mapping to correct one, and added implementation in code to flip up and down for the 16 layers. Unclear why this is necessary
</commit_message>
<xml_diff>
--- a/Tables/Grid_Wire_Channel_Mapping.xlsx
+++ b/Tables/Grid_Wire_Channel_Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/MultiGrid/MultiGridMux/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91D5ADB-B61A-9447-B4F0-143CFC0E4C3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8277B898-5D9A-6A49-B296-CA142187235A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="660" windowWidth="12140" windowHeight="16040" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
+    <workbookView xWindow="18120" yWindow="0" windowWidth="10680" windowHeight="18000" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81663BE0-29B8-F646-A110-AC508EA7B182}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,10 +457,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <v>15</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -469,10 +469,10 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -483,10 +483,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>14</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -495,10 +495,10 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -509,10 +509,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <v>13</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -521,10 +521,10 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -535,10 +535,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
         <v>12</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -547,10 +547,10 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -561,10 +561,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
         <v>11</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -573,10 +573,10 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -587,10 +587,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
         <v>10</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -599,10 +599,10 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -613,10 +613,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
         <v>9</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -625,10 +625,10 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9">
         <v>6</v>
@@ -639,10 +639,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
         <v>8</v>
-      </c>
-      <c r="B10">
-        <v>7</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -651,10 +651,10 @@
         <v>6</v>
       </c>
       <c r="E10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G10">
         <v>7</v>
@@ -665,10 +665,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
         <v>7</v>
-      </c>
-      <c r="B11">
-        <v>8</v>
       </c>
       <c r="C11">
         <v>8</v>
@@ -677,10 +677,10 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G11">
         <v>8</v>
@@ -691,10 +691,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
         <v>6</v>
-      </c>
-      <c r="B12">
-        <v>9</v>
       </c>
       <c r="C12">
         <v>9</v>
@@ -703,10 +703,10 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G12">
         <v>9</v>
@@ -717,10 +717,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
         <v>5</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -729,10 +729,10 @@
         <v>11</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G13">
         <v>10</v>
@@ -743,10 +743,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
         <v>4</v>
-      </c>
-      <c r="B14">
-        <v>11</v>
       </c>
       <c r="C14">
         <v>11</v>
@@ -755,10 +755,10 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G14">
         <v>11</v>
@@ -769,880 +769,877 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
         <v>3</v>
       </c>
-      <c r="B15">
+      <c r="E15">
         <v>12</v>
       </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
       <c r="F15">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
         <v>2</v>
       </c>
-      <c r="B16">
+      <c r="E16">
         <v>13</v>
       </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
       <c r="F16">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
         <v>1</v>
       </c>
-      <c r="B17">
+      <c r="E17">
         <v>14</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
       <c r="F17">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
         <v>0</v>
       </c>
-      <c r="B18">
+      <c r="E18">
         <v>15</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
       <c r="F18">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B19">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E19">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F19">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E20">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F20">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E21">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F21">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B22">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E22">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F22">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B23">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E23">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F23">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B24">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E24">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F24:F49" si="0">F8+16</f>
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B25">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E25">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F25">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B26">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E26">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F26">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B27">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E27">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F27">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B28">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E28">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F28">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B29">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E29">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E30">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B31">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E31">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f t="shared" ref="F24:F49" si="0">F15+16</f>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B32">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E32">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B33">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E33">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B34">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E34">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B35">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E35">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B36">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E36">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B37">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E37">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B38">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E38">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B39">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E39">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E40">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B41">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E41">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B42">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E42">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B43">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="E43">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B44">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E44">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B45">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="E45">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B46">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E46">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B47">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E47">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B48">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E48">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B49">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E49">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E50">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F50">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B51">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E51">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F51">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B52">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E52">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F52">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B53">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E53">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F53">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B54">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E54">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F54">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B55">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E55">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F55">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B56">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E56">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F56">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B57">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E57">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F57">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B58">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E58">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F58">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B59">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E59">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F59">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E60">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F60">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B61">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E61">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F61">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B62">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E62">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F62">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B63">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E63">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F63">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B64">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E64">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F64">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B65">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E65">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F65">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B66">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E66">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="F66">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B67">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B68">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B69">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B71">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B72">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B73">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B74">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B75">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B76">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B77">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B78">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
+        <v>76</v>
+      </c>
+      <c r="B79">
         <v>79</v>
-      </c>
-      <c r="B79">
-        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
+        <v>77</v>
+      </c>
+      <c r="B80">
         <v>78</v>
-      </c>
-      <c r="B80">
-        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
+        <v>78</v>
+      </c>
+      <c r="B81">
         <v>77</v>
-      </c>
-      <c r="B81">
-        <v>78</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
+        <v>79</v>
+      </c>
+      <c r="B82">
         <v>76</v>
-      </c>
-      <c r="B82">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>